<commit_message>
added scatter plot to bar plots
</commit_message>
<xml_diff>
--- a/raw_data/201113_Figure4Cbottom.xlsx
+++ b/raw_data/201113_Figure4Cbottom.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwnetid-my.sharepoint.com/personal/dalba_uw_edu/Documents/research/carothers/txtl data/BH4 and Co/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego Alba\Documents\GitHub\CRISPRai_Circuits_2021\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{AEF2F7AB-D554-A44D-BDF4-F25F2476F007}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C98B4768-E3F3-4576-8E82-099144AEC37E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B0B3935-08C1-4830-8CEE-8BF91E132533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{878F513D-B81F-5242-AE64-8F546998C009}"/>
+    <workbookView xWindow="10050" yWindow="3795" windowWidth="20295" windowHeight="14085" xr2:uid="{878F513D-B81F-5242-AE64-8F546998C009}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>pJF143.J3+085.J306</t>
   </si>
@@ -83,12 +83,6 @@
   <si>
     <t>RFP/OD600</t>
   </si>
-  <si>
-    <t>stdevs</t>
-  </si>
-  <si>
-    <t>Averages</t>
-  </si>
 </sst>
 </file>
 
@@ -130,7 +124,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -195,6 +191,14 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.44090599254309737"/>
+          <c:y val="0.43379249952236659"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -254,21 +258,6 @@
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
-                  <c:pt idx="0">
-                    <c:v>176.74217482065026</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>47.698222996250067</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>344.94245960208178</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>1.0605113546461105</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>576.11719363337852</c:v>
-                  </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
@@ -278,21 +267,6 @@
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
-                  <c:pt idx="0">
-                    <c:v>176.74217482065026</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>47.698222996250067</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>344.94245960208178</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>1.0605113546461105</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>576.11719363337852</c:v>
-                  </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:minus>
@@ -335,24 +309,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$6:$G$6</c:f>
+              <c:f>Sheet1!#REF!</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>11886.871333333334</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3104.0250000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>20712.130333333334</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>85.909333333333336</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>10675.550000000001</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1082,16 +1044,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>656166</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>93840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>298450</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>115005</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>189794</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1416,10 +1378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{010B5D12-CD6A-FC43-A82E-CC153674E28F}">
-  <dimension ref="A3:P6"/>
+  <dimension ref="A3:P22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="135" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:O1048576"/>
+    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3:Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1434,20 +1396,8 @@
       <c r="G3" t="s">
         <v>14</v>
       </c>
-      <c r="L3" t="s">
-        <v>12</v>
-      </c>
-      <c r="N3" t="s">
-        <v>13</v>
-      </c>
-      <c r="P3" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -1466,27 +1416,11 @@
       <c r="G4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K4" t="s">
-        <v>1</v>
-      </c>
-      <c r="L4" t="s">
-        <v>0</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="J4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
@@ -1507,65 +1441,159 @@
       <c r="G5" t="s">
         <v>10</v>
       </c>
-      <c r="K5" t="s">
-        <v>7</v>
-      </c>
-      <c r="L5" t="s">
-        <v>6</v>
-      </c>
-      <c r="M5" t="s">
-        <v>9</v>
-      </c>
-      <c r="N5" t="s">
-        <v>8</v>
-      </c>
-      <c r="O5" t="s">
-        <v>11</v>
-      </c>
-      <c r="P5" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="B6">
-        <v>294.03166666666664</v>
-      </c>
-      <c r="C6">
-        <v>11886.871333333334</v>
-      </c>
-      <c r="D6">
-        <v>3104.0250000000001</v>
-      </c>
-      <c r="E6">
-        <v>20712.130333333334</v>
-      </c>
-      <c r="F6">
-        <v>85.909333333333336</v>
-      </c>
-      <c r="G6">
-        <v>10675.550000000001</v>
-      </c>
-      <c r="K6">
-        <v>3.5513116356261003</v>
-      </c>
-      <c r="L6">
-        <v>176.74217482065026</v>
-      </c>
-      <c r="M6">
-        <v>47.698222996250067</v>
-      </c>
-      <c r="N6">
-        <v>344.94245960208178</v>
-      </c>
-      <c r="O6">
-        <v>1.0605113546461105</v>
-      </c>
-      <c r="P6">
-        <v>576.11719363337852</v>
-      </c>
+      <c r="B6" s="2">
+        <v>297.62599999999998</v>
+      </c>
+      <c r="C6" s="2">
+        <v>11951.401</v>
+      </c>
+      <c r="D6" s="2">
+        <v>3126.9940000000001</v>
+      </c>
+      <c r="E6" s="2">
+        <v>20573.683000000001</v>
+      </c>
+      <c r="F6" s="2">
+        <v>86.966999999999999</v>
+      </c>
+      <c r="G6" s="2">
+        <v>11164.51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B7" s="2">
+        <v>293.94400000000002</v>
+      </c>
+      <c r="C7" s="2">
+        <v>12022.281000000001</v>
+      </c>
+      <c r="D7" s="2">
+        <v>3049.1880000000001</v>
+      </c>
+      <c r="E7" s="2">
+        <v>20457.919999999998</v>
+      </c>
+      <c r="F7" s="2">
+        <v>84.846000000000004</v>
+      </c>
+      <c r="G7" s="2">
+        <v>10040.43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
+        <v>290.52499999999998</v>
+      </c>
+      <c r="C8" s="2">
+        <v>11686.932000000001</v>
+      </c>
+      <c r="D8" s="2">
+        <v>3135.893</v>
+      </c>
+      <c r="E8" s="2">
+        <v>21104.788</v>
+      </c>
+      <c r="F8" s="2">
+        <v>85.915000000000006</v>
+      </c>
+      <c r="G8" s="2">
+        <v>10821.71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>